<commit_message>
Get 2020 spreadsheet templates
</commit_message>
<xml_diff>
--- a/public/templates/MER-template.xlsx
+++ b/public/templates/MER-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -91,13 +91,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="120">
   <si>
-    <t xml:space="preserve">2018-2019 MINISTRY EXPENSE REIMBURSEMENT</t>
+    <t xml:space="preserve">2019-2020 MINISTRY EXPENSE REIMBURSEMENT</t>
   </si>
   <si>
     <t xml:space="preserve">For WBT Canada Directed Personnel on Canada Payroll only</t>
   </si>
   <si>
-    <t xml:space="preserve">Revised for April 2019</t>
+    <t xml:space="preserve">Revised for January 2020</t>
   </si>
   <si>
     <t xml:space="preserve">Last Name:</t>
@@ -1340,8 +1340,8 @@
   </sheetPr>
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2779,7 +2779,7 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Get updated MER template for April 2021
</commit_message>
<xml_diff>
--- a/public/templates/MER-template.xlsx
+++ b/public/templates/MER-template.xlsx
@@ -34,6 +34,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">5oooo series number 
 Ask office if red doesn't clear</t>
@@ -48,6 +49,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Please contact mer@wycliffe.ca for details
 </t>
@@ -62,6 +64,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Amount released to member 
 to pay for moving expenses
@@ -77,6 +80,7 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Enter 3 letter month and 4 digit year
 Will appear in cell as:    Mmm yy
@@ -91,13 +95,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="120">
   <si>
-    <t xml:space="preserve">2019-2020 MINISTRY EXPENSE REIMBURSEMENT</t>
+    <t xml:space="preserve">2020-2021 MINISTRY EXPENSE REIMBURSEMENT</t>
   </si>
   <si>
     <t xml:space="preserve">For WBT Canada Directed Personnel on Canada Payroll only</t>
   </si>
   <si>
-    <t xml:space="preserve">Revised for January 2020</t>
+    <t xml:space="preserve">Revised for April 2021</t>
   </si>
   <si>
     <t xml:space="preserve">Last Name:</t>
@@ -415,6 +419,7 @@
         <sz val="11"/>
         <rFont val="Cambria"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Purchase Date </t>
     </r>
@@ -423,6 +428,7 @@
         <sz val="11"/>
         <rFont val="Cambria"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(d Mmm 'yy)</t>
     </r>
@@ -473,19 +479,20 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="MMM\-YY"/>
+    <numFmt numFmtId="165" formatCode="MMM/YY"/>
     <numFmt numFmtId="166" formatCode="MMM\ YY"/>
-    <numFmt numFmtId="167" formatCode="D\-MMM\-YY"/>
+    <numFmt numFmtId="167" formatCode="D/MMM/YY"/>
     <numFmt numFmtId="168" formatCode="@"/>
-    <numFmt numFmtId="169" formatCode="&quot; $&quot;* #,##0.00\ ;&quot; $&quot;* \(#,##0.00\);&quot; $&quot;* \-#\ ;\ @\ "/>
+    <numFmt numFmtId="169" formatCode="&quot; $&quot;* #,##0.00\ ;&quot; $&quot;* \(#,##0.00\);&quot; $&quot;* \-#\ ;@\ "/>
     <numFmt numFmtId="170" formatCode="\$#,##0.00"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -504,108 +511,36 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -613,17 +548,20 @@
       <color rgb="FFDCCE9C"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial Narrow"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -631,18 +569,21 @@
       <color rgb="FFDCCE9C"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFDCCE9C"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -650,18 +591,21 @@
       <color rgb="FFB71509"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFB71509"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -669,15 +613,17 @@
       <color rgb="FFDCCE9C"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Inconsolata"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -686,50 +632,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFB71509"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF76923C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFD6E3BC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD6E3BC"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFC2D69B"/>
       </patternFill>
     </fill>
     <fill>
@@ -741,13 +645,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF4F6128"/>
-        <bgColor rgb="FF333333"/>
+        <bgColor rgb="FF666699"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF9BBB59"/>
-        <bgColor rgb="FFC2D69B"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
     <fill>
@@ -775,27 +679,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -855,7 +744,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -879,423 +768,355 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="78">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="12" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="13" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="19" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="14" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="19" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="14" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="19" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="14" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="19" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="25" fillId="14" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="25" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="14" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="14" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="27" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="14" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="18" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="24" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="18" fillId="14" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="12" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="18" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="22" fillId="9" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="22" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="18" fillId="12" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF978235"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC2D69B"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF76923C"/>
       <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFD6E3BC"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1306,20 +1127,20 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFDCCE9C"/>
+      <rgbColor rgb="FFD6E3BC"/>
+      <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFDCCE9C"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF9BBB59"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF4F6128"/>
-      <rgbColor rgb="FF76923C"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -1327,7 +1148,7 @@
       <rgbColor rgb="FFB71509"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF4F6128"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1341,7 +1162,7 @@
   <dimension ref="A1:L68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2792,7 +2613,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.29"/>

</xml_diff>